<commit_message>
HUBO UN CONFLICTO INTENTO ARREGLAR, JE
</commit_message>
<xml_diff>
--- a/df.xlsx
+++ b/df.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="206">
   <si>
     <t xml:space="preserve">fecha</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">cau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turb</t>
   </si>
   <si>
     <t xml:space="preserve">coment</t>
@@ -851,13 +854,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT29"/>
+  <dimension ref="A1:AU29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC27" activeCellId="0" sqref="AC27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.01"/>
@@ -882,19 +885,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="7.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="84.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="50.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="193.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="34.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="16.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="25.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="6.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="84.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="50.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="193.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="34.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="16.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="25.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="6.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,16 +1040,19 @@
       <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>45410</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -1066,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>-31.072472</v>
@@ -1123,31 +1130,31 @@
         <f aca="false">AD2*AE2*AF2</f>
         <v>0.547638</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="AI2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="AJ2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AK2" s="1" t="n">
+      <c r="AK2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL2" s="1" t="n">
         <v>334054834</v>
       </c>
-      <c r="AL2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM2" s="3" t="n">
+      <c r="AM2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" s="3" t="n">
         <v>45410.6502893519</v>
       </c>
-      <c r="AP2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AT2" s="1" t="n">
+      <c r="AS2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1156,10 +1163,10 @@
         <v>45434</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0</v>
@@ -1180,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>-31.158276</v>
@@ -1237,28 +1244,28 @@
         <f aca="false">AD3*AE3*AF3</f>
         <v>0.25</v>
       </c>
-      <c r="AI3" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="AJ3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AK3" s="1" t="n">
+      <c r="AK3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL3" s="1" t="n">
         <v>341790028</v>
       </c>
-      <c r="AL3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM3" s="3" t="n">
+      <c r="AM3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN3" s="3" t="n">
         <v>45434.9321064815</v>
       </c>
-      <c r="AP3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AT3" s="1" t="n">
+      <c r="AS3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1267,10 +1274,10 @@
         <v>45434</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
@@ -1291,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>-31.158275</v>
@@ -1339,28 +1346,28 @@
         <f aca="false">AD4*AE4*AF4</f>
         <v>0</v>
       </c>
-      <c r="AI4" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AJ4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AK4" s="1" t="n">
+      <c r="AK4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL4" s="1" t="n">
         <v>341790143</v>
       </c>
-      <c r="AL4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM4" s="3" t="n">
+      <c r="AM4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN4" s="3" t="n">
         <v>45434.9326736111</v>
       </c>
-      <c r="AP4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AT4" s="1" t="n">
+      <c r="AS4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU4" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1369,10 +1376,10 @@
         <v>45434</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -1393,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>-31.158269</v>
@@ -1420,28 +1427,28 @@
         <f aca="false">AD5*AE5*AF5</f>
         <v>0</v>
       </c>
-      <c r="AI5" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="AJ5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AK5" s="1" t="n">
+      <c r="AK5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL5" s="1" t="n">
         <v>341792512</v>
       </c>
-      <c r="AL5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM5" s="3" t="n">
+      <c r="AM5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN5" s="3" t="n">
         <v>45434.9438078704</v>
       </c>
-      <c r="AP5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR5" s="1" t="s">
+      <c r="AQ5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AT5" s="1" t="n">
+      <c r="AS5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU5" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1450,10 +1457,10 @@
         <v>45434</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>
@@ -1474,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>-31.158269</v>
@@ -1501,28 +1508,28 @@
         <f aca="false">AD6*AE6*AF6</f>
         <v>0</v>
       </c>
-      <c r="AI6" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AJ6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AK6" s="1" t="n">
+      <c r="AK6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL6" s="1" t="n">
         <v>341792614</v>
       </c>
-      <c r="AL6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AM6" s="3" t="n">
+      <c r="AM6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN6" s="3" t="n">
         <v>45434.9442708333</v>
       </c>
-      <c r="AP6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR6" s="1" t="s">
+      <c r="AQ6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AT6" s="1" t="n">
+      <c r="AS6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU6" s="1" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1531,10 +1538,10 @@
         <v>45434</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
@@ -1555,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K7" s="1" t="n">
         <v>-31.15827</v>
@@ -1582,28 +1589,28 @@
         <f aca="false">AD7*AE7*AF7</f>
         <v>0</v>
       </c>
-      <c r="AI7" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="AJ7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AK7" s="1" t="n">
+      <c r="AK7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL7" s="1" t="n">
         <v>341792645</v>
       </c>
-      <c r="AL7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM7" s="3" t="n">
+      <c r="AM7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN7" s="3" t="n">
         <v>45434.9443981481</v>
       </c>
-      <c r="AP7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR7" s="1" t="s">
+      <c r="AQ7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AT7" s="1" t="n">
+      <c r="AS7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU7" s="1" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1612,10 +1619,10 @@
         <v>45434</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0</v>
@@ -1636,7 +1643,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>-31.158269</v>
@@ -1663,28 +1670,28 @@
         <f aca="false">AD8*AE8*AF8</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="AJ8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AK8" s="1" t="n">
+      <c r="AK8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL8" s="1" t="n">
         <v>341792677</v>
       </c>
-      <c r="AL8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM8" s="3" t="n">
+      <c r="AM8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN8" s="3" t="n">
         <v>45434.9445138889</v>
       </c>
-      <c r="AP8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR8" s="1" t="s">
+      <c r="AQ8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AT8" s="1" t="n">
+      <c r="AS8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU8" s="1" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1693,10 +1700,10 @@
         <v>45442</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0</v>
@@ -1717,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K9" s="1" t="n">
         <v>-31.063232</v>
@@ -1786,28 +1793,28 @@
         <f aca="false">AD9*AE9*AF9</f>
         <v>0.2632014</v>
       </c>
-      <c r="AI9" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AJ9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AK9" s="1" t="n">
+      <c r="AK9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL9" s="1" t="n">
         <v>344327312</v>
       </c>
-      <c r="AL9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM9" s="3" t="n">
+      <c r="AM9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN9" s="3" t="n">
         <v>45442.5702546296</v>
       </c>
-      <c r="AP9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT9" s="1" t="n">
+      <c r="AQ9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU9" s="1" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1816,10 +1823,10 @@
         <v>45442</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>0</v>
@@ -1840,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K10" s="1" t="n">
         <v>-31.068288</v>
@@ -1909,28 +1916,28 @@
         <f aca="false">AD10*AE10*AF10</f>
         <v>0.295869</v>
       </c>
-      <c r="AI10" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="AJ10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AK10" s="1" t="n">
+      <c r="AK10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL10" s="1" t="n">
         <v>344349155</v>
       </c>
-      <c r="AL10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AM10" s="3" t="n">
+      <c r="AM10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN10" s="3" t="n">
         <v>45442.6042013889</v>
       </c>
-      <c r="AP10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR10" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT10" s="1" t="n">
+      <c r="AQ10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU10" s="1" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1939,10 +1946,10 @@
         <v>45442</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0</v>
@@ -1963,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K11" s="1" t="n">
         <v>-31.072632</v>
@@ -2026,28 +2033,28 @@
         <f aca="false">AD11*AE11*AF11</f>
         <v>0.357553875</v>
       </c>
-      <c r="AI11" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="AJ11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AK11" s="1" t="n">
+      <c r="AK11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL11" s="1" t="n">
         <v>344365235</v>
       </c>
-      <c r="AL11" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AM11" s="3" t="n">
+      <c r="AM11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AN11" s="3" t="n">
         <v>45442.6313657407</v>
       </c>
-      <c r="AP11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT11" s="1" t="n">
+      <c r="AQ11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU11" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -2056,10 +2063,10 @@
         <v>45442</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -2080,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K12" s="1" t="n">
         <v>-31.076567</v>
@@ -2143,28 +2150,28 @@
         <f aca="false">AD12*AE12*AF12</f>
         <v>0.42471</v>
       </c>
-      <c r="AI12" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="AJ12" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AK12" s="1" t="n">
+      <c r="AK12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL12" s="1" t="n">
         <v>344403932</v>
       </c>
-      <c r="AL12" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AM12" s="3" t="n">
+      <c r="AM12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN12" s="3" t="n">
         <v>45442.701400463</v>
       </c>
-      <c r="AP12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT12" s="1" t="n">
+      <c r="AQ12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU12" s="1" t="n">
         <v>11</v>
       </c>
     </row>
@@ -2173,10 +2180,10 @@
         <v>45417</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0</v>
@@ -2197,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>-31.007081</v>
@@ -2263,31 +2270,31 @@
         <f aca="false">AD13*AE13*AF13</f>
         <v>0.47616</v>
       </c>
-      <c r="AH13" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="AI13" s="1" t="s">
         <v>113</v>
       </c>
       <c r="AJ13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AK13" s="1" t="n">
+      <c r="AK13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL13" s="1" t="n">
         <v>346656440</v>
       </c>
-      <c r="AL13" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AM13" s="3" t="n">
+      <c r="AM13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AN13" s="3" t="n">
         <v>45449.8028240741</v>
       </c>
-      <c r="AP13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT13" s="1" t="n">
+      <c r="AQ13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU13" s="1" t="n">
         <v>12</v>
       </c>
     </row>
@@ -2296,10 +2303,10 @@
         <v>45417</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0</v>
@@ -2320,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K14" s="1" t="n">
         <v>-31.00637</v>
@@ -2386,31 +2393,31 @@
         <f aca="false">AD14*AE14*AF14</f>
         <v>0.588992625</v>
       </c>
-      <c r="AH14" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="AI14" s="1" t="s">
         <v>119</v>
       </c>
       <c r="AJ14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AK14" s="1" t="n">
+      <c r="AK14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL14" s="1" t="n">
         <v>347858608</v>
       </c>
-      <c r="AL14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AM14" s="3" t="n">
+      <c r="AM14" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN14" s="3" t="n">
         <v>45453.8937268519</v>
       </c>
-      <c r="AP14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AT14" s="1" t="n">
+      <c r="AQ14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AU14" s="1" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2419,10 +2426,10 @@
         <v>45632</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
@@ -2443,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K15" s="1" t="n">
         <v>-31.062945</v>
@@ -2512,28 +2519,28 @@
         <f aca="false">AD15*AE15*AF15</f>
         <v>0.29988</v>
       </c>
-      <c r="AI15" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="AJ15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AK15" s="1" t="n">
+      <c r="AK15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL15" s="1" t="n">
         <v>419735374</v>
       </c>
-      <c r="AL15" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AM15" s="3" t="n">
+      <c r="AM15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN15" s="3" t="n">
         <v>45638.7180208333</v>
       </c>
-      <c r="AP15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AT15" s="1" t="n">
+      <c r="AQ15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AU15" s="1" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2542,10 +2549,10 @@
         <v>45632</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -2566,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K16" s="1" t="n">
         <v>-31.063085</v>
@@ -2638,28 +2645,28 @@
         <f aca="false">AD16*AE16*AF16</f>
         <v>0.4818294</v>
       </c>
-      <c r="AI16" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="AJ16" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AK16" s="1" t="n">
+      <c r="AK16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL16" s="1" t="n">
         <v>419737711</v>
       </c>
-      <c r="AL16" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AM16" s="3" t="n">
+      <c r="AM16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN16" s="3" t="n">
         <v>45638.7223958333</v>
       </c>
-      <c r="AP16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AT16" s="1" t="n">
+      <c r="AQ16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AU16" s="1" t="n">
         <v>15</v>
       </c>
     </row>
@@ -2668,10 +2675,10 @@
         <v>45632</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
@@ -2692,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K17" s="1" t="n">
         <v>-31.07665</v>
@@ -2764,28 +2771,28 @@
         <f aca="false">AD17*AE17*AF17</f>
         <v>0.6359535</v>
       </c>
-      <c r="AI17" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="AJ17" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AK17" s="1" t="n">
+      <c r="AK17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL17" s="1" t="n">
         <v>419739274</v>
       </c>
-      <c r="AL17" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM17" s="3" t="n">
+      <c r="AM17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN17" s="3" t="n">
         <v>45638.7253935185</v>
       </c>
-      <c r="AP17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AT17" s="1" t="n">
+      <c r="AQ17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AU17" s="1" t="n">
         <v>16</v>
       </c>
     </row>
@@ -2794,10 +2801,10 @@
         <v>45632</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0</v>
@@ -2818,7 +2825,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K18" s="1" t="n">
         <v>-31.081685</v>
@@ -2890,31 +2897,31 @@
         <f aca="false">AD18*AE18*AF18</f>
         <v>0.3244723</v>
       </c>
-      <c r="AH18" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="AI18" s="1" t="s">
         <v>142</v>
       </c>
       <c r="AJ18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AK18" s="1" t="n">
+      <c r="AK18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL18" s="1" t="n">
         <v>419740828</v>
       </c>
-      <c r="AL18" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AM18" s="3" t="n">
+      <c r="AM18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN18" s="3" t="n">
         <v>45638.7281828704</v>
       </c>
-      <c r="AP18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR18" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AT18" s="1" t="n">
+      <c r="AQ18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AU18" s="1" t="n">
         <v>17</v>
       </c>
     </row>
@@ -2923,10 +2930,10 @@
         <v>45632</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0</v>
@@ -2947,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K19" s="1" t="n">
         <v>-31.072685</v>
@@ -3016,28 +3023,28 @@
         <f aca="false">AD19*AE19*AF19</f>
         <v>0.4817904</v>
       </c>
-      <c r="AI19" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="AJ19" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AK19" s="1" t="n">
+      <c r="AK19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL19" s="1" t="n">
         <v>419749907</v>
       </c>
-      <c r="AL19" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AM19" s="3" t="n">
+      <c r="AM19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN19" s="3" t="n">
         <v>45638.7450462963</v>
       </c>
-      <c r="AP19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR19" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AT19" s="1" t="n">
+      <c r="AQ19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AU19" s="1" t="n">
         <v>18</v>
       </c>
     </row>
@@ -3046,10 +3053,10 @@
         <v>45541</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -3070,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K20" s="1" t="n">
         <v>-31.06294</v>
@@ -3142,28 +3149,28 @@
         <f aca="false">AD20*AE20*AF20</f>
         <v>0.0790296</v>
       </c>
-      <c r="AI20" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="AJ20" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AK20" s="1" t="n">
+      <c r="AK20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AL20" s="1" t="n">
         <v>420032406</v>
       </c>
-      <c r="AL20" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="AM20" s="3" t="n">
+      <c r="AM20" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN20" s="3" t="n">
         <v>45639.5085532407</v>
       </c>
-      <c r="AP20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR20" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT20" s="1" t="n">
+      <c r="AQ20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU20" s="1" t="n">
         <v>19</v>
       </c>
     </row>
@@ -3172,10 +3179,10 @@
         <v>45541</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>0</v>
@@ -3196,7 +3203,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K21" s="1" t="n">
         <v>-31.081662</v>
@@ -3268,31 +3275,31 @@
         <f aca="false">AD21*AE21*AF21</f>
         <v>0.142324</v>
       </c>
-      <c r="AH21" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="AI21" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AJ21" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AK21" s="1" t="n">
+      <c r="AK21" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL21" s="1" t="n">
         <v>420039666</v>
       </c>
-      <c r="AL21" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="AM21" s="3" t="n">
+      <c r="AM21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN21" s="3" t="n">
         <v>45639.5212847222</v>
       </c>
-      <c r="AP21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR21" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT21" s="1" t="n">
+      <c r="AQ21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU21" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3301,10 +3308,10 @@
         <v>45541</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>0</v>
@@ -3325,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K22" s="1" t="n">
         <v>-31.06841</v>
@@ -3397,28 +3404,28 @@
         <f aca="false">AD22*AE22*AF22</f>
         <v>0.1954953</v>
       </c>
-      <c r="AI22" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="AJ22" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="AK22" s="1" t="n">
+      <c r="AK22" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AL22" s="1" t="n">
         <v>420041286</v>
       </c>
-      <c r="AL22" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM22" s="3" t="n">
+      <c r="AM22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AN22" s="3" t="n">
         <v>45639.5242013889</v>
       </c>
-      <c r="AP22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR22" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT22" s="1" t="n">
+      <c r="AQ22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU22" s="1" t="n">
         <v>21</v>
       </c>
     </row>
@@ -3427,10 +3434,10 @@
         <v>45541</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>0</v>
@@ -3451,7 +3458,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K23" s="1" t="n">
         <v>-31.072531</v>
@@ -3523,28 +3530,28 @@
         <f aca="false">AD23*AE23*AF23</f>
         <v>0.2250972</v>
       </c>
-      <c r="AI23" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="AJ23" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AK23" s="1" t="n">
+      <c r="AK23" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL23" s="1" t="n">
         <v>420044475</v>
       </c>
-      <c r="AL23" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="AM23" s="3" t="n">
+      <c r="AM23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AN23" s="3" t="n">
         <v>45639.5299768519</v>
       </c>
-      <c r="AP23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR23" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT23" s="1" t="n">
+      <c r="AQ23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU23" s="1" t="n">
         <v>22</v>
       </c>
     </row>
@@ -3553,10 +3560,10 @@
         <v>45541</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -3577,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K24" s="1" t="n">
         <v>-31.076678</v>
@@ -3649,31 +3656,31 @@
         <f aca="false">AD24*AE24*AF24</f>
         <v>0.1866788</v>
       </c>
-      <c r="AH24" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="AI24" s="1" t="s">
         <v>175</v>
       </c>
       <c r="AJ24" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AK24" s="1" t="n">
+      <c r="AK24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL24" s="1" t="n">
         <v>420047258</v>
       </c>
-      <c r="AL24" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="AM24" s="3" t="n">
+      <c r="AM24" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN24" s="3" t="n">
         <v>45639.5344097222</v>
       </c>
-      <c r="AP24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR24" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AT24" s="1" t="n">
+      <c r="AQ24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS24" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU24" s="1" t="n">
         <v>23</v>
       </c>
     </row>
@@ -3682,10 +3689,10 @@
         <v>45723</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>1</v>
@@ -3706,7 +3713,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K25" s="1" t="n">
         <v>-31.0765966</v>
@@ -3775,28 +3782,28 @@
         <f aca="false">AD25*AE25*AF25</f>
         <v>0.6370221</v>
       </c>
-      <c r="AI25" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="AJ25" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AK25" s="1" t="n">
+      <c r="AK25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL25" s="1" t="n">
         <v>452082664</v>
       </c>
-      <c r="AL25" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AM25" s="3" t="n">
+      <c r="AM25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AN25" s="3" t="n">
         <v>45730.7853356482</v>
       </c>
-      <c r="AP25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR25" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AT25" s="1" t="n">
+      <c r="AQ25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS25" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AU25" s="1" t="n">
         <v>24</v>
       </c>
     </row>
@@ -3805,10 +3812,10 @@
         <v>45723</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>0</v>
@@ -3829,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K26" s="1" t="n">
         <v>-31.072944</v>
@@ -3901,31 +3908,31 @@
         <f aca="false">AD26*AE26*AF26</f>
         <v>0.3663662625</v>
       </c>
-      <c r="AH26" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="AI26" s="1" t="s">
         <v>186</v>
       </c>
       <c r="AJ26" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AK26" s="1" t="n">
+      <c r="AK26" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AL26" s="1" t="n">
         <v>452091792</v>
       </c>
-      <c r="AL26" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM26" s="3" t="n">
+      <c r="AM26" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AN26" s="3" t="n">
         <v>45730.8057291667</v>
       </c>
-      <c r="AP26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR26" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AT26" s="1" t="n">
+      <c r="AQ26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS26" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AU26" s="1" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3934,10 +3941,10 @@
         <v>45723</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>0</v>
@@ -3958,7 +3965,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K27" s="1" t="n">
         <v>-31.068312</v>
@@ -4030,31 +4037,31 @@
         <f aca="false">AD27*AE27*AF27</f>
         <v>0.2306275712</v>
       </c>
-      <c r="AH27" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="AI27" s="1" t="s">
         <v>192</v>
       </c>
       <c r="AJ27" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AK27" s="1" t="n">
+      <c r="AK27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL27" s="1" t="n">
         <v>452095654</v>
       </c>
-      <c r="AL27" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AM27" s="3" t="n">
+      <c r="AM27" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AN27" s="3" t="n">
         <v>45730.8156481482</v>
       </c>
-      <c r="AP27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR27" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AT27" s="1" t="n">
+      <c r="AQ27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS27" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AU27" s="1" t="n">
         <v>26</v>
       </c>
     </row>
@@ -4063,10 +4070,10 @@
         <v>45723</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>0</v>
@@ -4087,7 +4094,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K28" s="1" t="n">
         <v>-31.081699</v>
@@ -4156,31 +4163,31 @@
         <f aca="false">AD28*AE28*AF28</f>
         <v>0.412040464375</v>
       </c>
-      <c r="AH28" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="AI28" s="1" t="s">
         <v>198</v>
       </c>
       <c r="AJ28" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="AK28" s="1" t="n">
+      <c r="AK28" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL28" s="1" t="n">
         <v>453036628</v>
       </c>
-      <c r="AL28" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AM28" s="3" t="n">
+      <c r="AM28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN28" s="3" t="n">
         <v>45733.7454513889</v>
       </c>
-      <c r="AP28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR28" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AT28" s="1" t="n">
+      <c r="AQ28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS28" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AU28" s="1" t="n">
         <v>27</v>
       </c>
     </row>
@@ -4189,10 +4196,10 @@
         <v>45723</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>0</v>
@@ -4213,7 +4220,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K29" s="1" t="n">
         <v>-31.063145</v>
@@ -4285,28 +4292,28 @@
         <f aca="false">AD29*AE29*AF29</f>
         <v>0.09963078125</v>
       </c>
-      <c r="AI29" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="AJ29" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AK29" s="1" t="n">
+      <c r="AK29" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AL29" s="1" t="n">
         <v>453040308</v>
       </c>
-      <c r="AL29" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AM29" s="3" t="n">
+      <c r="AM29" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN29" s="3" t="n">
         <v>45733.7528472222</v>
       </c>
-      <c r="AP29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR29" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AT29" s="1" t="n">
+      <c r="AQ29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS29" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AU29" s="1" t="n">
         <v>28</v>
       </c>
     </row>

</xml_diff>